<commit_message>
sua chuc nang tao lo tai khoan
</commit_message>
<xml_diff>
--- a/server/src/main/resources/static/account_create_sample.xlsx
+++ b/server/src/main/resources/static/account_create_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School_DL\dean\server\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE2CCAF-530E-4038-AE81-949FED33F034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B96BEA-48B8-4305-81EB-0A8DC40EB824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,11 +93,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,18 +382,18 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.69140625" customWidth="1"/>
-    <col min="2" max="2" width="18.23046875" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="19.07421875" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>